<commit_message>
fixed sample for Talbe S4a, S5a
</commit_message>
<xml_diff>
--- a/Tables/Table_S4.xlsx
+++ b/Tables/Table_S4.xlsx
@@ -415,14 +415,14 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>-0.571</t>
+          <t>-0.883</t>
         </is>
       </c>
       <c r="F2">
-        <v>-1.188</v>
+        <v>-1.471</v>
       </c>
       <c r="G2">
-        <v>0.006</v>
+        <v>-0.29</v>
       </c>
     </row>
     <row r="3">
@@ -446,14 +446,14 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>-0.715</t>
+          <t>-0.283</t>
         </is>
       </c>
       <c r="F3">
-        <v>-1.518</v>
+        <v>-1.194</v>
       </c>
       <c r="G3">
-        <v>0.122</v>
+        <v>0.606</v>
       </c>
     </row>
     <row r="4">
@@ -477,14 +477,14 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.222</t>
+          <t>0.009</t>
         </is>
       </c>
       <c r="F4">
-        <v>-0.373</v>
+        <v>-0.644</v>
       </c>
       <c r="G4">
-        <v>0.821</v>
+        <v>0.677</v>
       </c>
     </row>
     <row r="5">
@@ -508,14 +508,14 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.034</t>
+          <t>0.204</t>
         </is>
       </c>
       <c r="F5">
-        <v>-0.769</v>
+        <v>-0.671</v>
       </c>
       <c r="G5">
-        <v>0.828</v>
+        <v>1.059</v>
       </c>
     </row>
     <row r="6">
@@ -539,7 +539,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>21%</t>
+          <t>98%</t>
         </is>
       </c>
     </row>
@@ -564,7 +564,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>79%</t>
+          <t>2%</t>
         </is>
       </c>
     </row>
@@ -589,14 +589,14 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>-0.577</t>
+          <t>-0.568</t>
         </is>
       </c>
       <c r="F8">
-        <v>-1.692</v>
+        <v>-1.72</v>
       </c>
       <c r="G8">
-        <v>0.539</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="9">
@@ -620,14 +620,14 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.284</t>
+          <t>0.263</t>
         </is>
       </c>
       <c r="F9">
-        <v>-1.234</v>
+        <v>-1.181</v>
       </c>
       <c r="G9">
-        <v>1.752</v>
+        <v>1.766</v>
       </c>
     </row>
     <row r="10">
@@ -651,14 +651,14 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>-0.522</t>
+          <t>-0.548</t>
         </is>
       </c>
       <c r="F10">
-        <v>-1.758</v>
+        <v>-1.802</v>
       </c>
       <c r="G10">
-        <v>0.679</v>
+        <v>0.643</v>
       </c>
     </row>
     <row r="11">
@@ -682,14 +682,14 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.096</t>
+          <t>1.12</t>
         </is>
       </c>
       <c r="F11">
-        <v>-0.642</v>
+        <v>-0.576</v>
       </c>
       <c r="G11">
-        <v>2.803</v>
+        <v>2.873</v>
       </c>
     </row>
     <row r="12">
@@ -763,14 +763,14 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1.547</t>
+          <t>1.542</t>
         </is>
       </c>
       <c r="F14">
-        <v>1.099</v>
+        <v>1.102</v>
       </c>
       <c r="G14">
-        <v>1.984</v>
+        <v>1.985</v>
       </c>
     </row>
     <row r="15">
@@ -794,14 +794,14 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>0.29</t>
+          <t>0.289</t>
         </is>
       </c>
       <c r="F15">
-        <v>-0.327</v>
+        <v>-0.308</v>
       </c>
       <c r="G15">
-        <v>0.913</v>
+        <v>0.892</v>
       </c>
     </row>
     <row r="16">
@@ -825,14 +825,14 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>0.587</t>
+          <t>0.595</t>
         </is>
       </c>
       <c r="F16">
-        <v>0.208</v>
+        <v>0.218</v>
       </c>
       <c r="G16">
-        <v>0.951</v>
+        <v>0.968</v>
       </c>
     </row>
     <row r="17">
@@ -856,14 +856,14 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.23</t>
+          <t>0.229</t>
         </is>
       </c>
       <c r="F17">
-        <v>-0.166</v>
+        <v>-0.175</v>
       </c>
       <c r="G17">
-        <v>0.64</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="18">
@@ -887,14 +887,14 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>-0.645</t>
+          <t>-0.653</t>
         </is>
       </c>
       <c r="F18">
-        <v>-1.137</v>
+        <v>-1.151</v>
       </c>
       <c r="G18">
-        <v>-0.125</v>
+        <v>-0.152</v>
       </c>
     </row>
     <row r="19">
@@ -918,14 +918,14 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>-0.026</t>
+          <t>-0.029</t>
         </is>
       </c>
       <c r="F19">
-        <v>-0.5679999999999999</v>
+        <v>-0.547</v>
       </c>
       <c r="G19">
-        <v>0.497</v>
+        <v>0.508</v>
       </c>
     </row>
     <row r="20">
@@ -1044,14 +1044,14 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>1.64</t>
+          <t>1.637</t>
         </is>
       </c>
       <c r="F24">
-        <v>1.378</v>
+        <v>1.368</v>
       </c>
       <c r="G24">
-        <v>1.909</v>
+        <v>1.893</v>
       </c>
     </row>
     <row r="25">
@@ -1075,14 +1075,14 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>-0.407</t>
+          <t>-0.4</t>
         </is>
       </c>
       <c r="F25">
-        <v>-0.786</v>
+        <v>-0.772</v>
       </c>
       <c r="G25">
-        <v>-0.028</v>
+        <v>-0.026</v>
       </c>
     </row>
     <row r="26">
@@ -1106,14 +1106,14 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>0.492</t>
+          <t>0.494</t>
         </is>
       </c>
       <c r="F26">
-        <v>0.196</v>
+        <v>0.2</v>
       </c>
       <c r="G26">
-        <v>0.787</v>
+        <v>0.788</v>
       </c>
     </row>
     <row r="27">
@@ -1141,10 +1141,10 @@
         </is>
       </c>
       <c r="F27">
-        <v>-0.202</v>
+        <v>-0.208</v>
       </c>
       <c r="G27">
-        <v>0.33</v>
+        <v>0.332</v>
       </c>
     </row>
     <row r="28">
@@ -1168,14 +1168,14 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>0.059</t>
+          <t>0.051</t>
         </is>
       </c>
       <c r="F28">
-        <v>-0.335</v>
+        <v>-0.355</v>
       </c>
       <c r="G28">
-        <v>0.444</v>
+        <v>0.453</v>
       </c>
     </row>
     <row r="29">
@@ -1199,14 +1199,14 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>0.194</t>
+          <t>0.201</t>
         </is>
       </c>
       <c r="F29">
-        <v>-0.165</v>
+        <v>-0.183</v>
       </c>
       <c r="G29">
-        <v>0.573</v>
+        <v>0.58</v>
       </c>
     </row>
     <row r="30">
@@ -1325,14 +1325,14 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>0.514</t>
+          <t>0.508</t>
         </is>
       </c>
       <c r="F34">
-        <v>0.218</v>
+        <v>0.209</v>
       </c>
       <c r="G34">
-        <v>0.8169999999999999</v>
+        <v>0.8070000000000001</v>
       </c>
     </row>
     <row r="35">
@@ -1356,11 +1356,11 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>-0.097</t>
+          <t>-0.09</t>
         </is>
       </c>
       <c r="F35">
-        <v>-0.539</v>
+        <v>-0.524</v>
       </c>
       <c r="G35">
         <v>0.327</v>
@@ -1387,14 +1387,14 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>0.141</t>
+          <t>0.138</t>
         </is>
       </c>
       <c r="F36">
-        <v>-0.108</v>
+        <v>-0.107</v>
       </c>
       <c r="G36">
-        <v>0.391</v>
+        <v>0.385</v>
       </c>
     </row>
     <row r="37">
@@ -1418,14 +1418,14 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>0.079</t>
+          <t>0.086</t>
         </is>
       </c>
       <c r="F37">
-        <v>-0.179</v>
+        <v>-0.171</v>
       </c>
       <c r="G37">
-        <v>0.336</v>
+        <v>0.347</v>
       </c>
     </row>
     <row r="38">
@@ -1449,14 +1449,14 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>-0.148</t>
+          <t>-0.145</t>
         </is>
       </c>
       <c r="F38">
-        <v>-0.503</v>
+        <v>-0.477</v>
       </c>
       <c r="G38">
-        <v>0.196</v>
+        <v>0.206</v>
       </c>
     </row>
     <row r="39">
@@ -1480,14 +1480,14 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>0.004</t>
+          <t>0.001</t>
         </is>
       </c>
       <c r="F39">
-        <v>-0.366</v>
+        <v>-0.357</v>
       </c>
       <c r="G39">
-        <v>0.367</v>
+        <v>0.356</v>
       </c>
     </row>
     <row r="40">

</xml_diff>